<commit_message>
REPORTGEN-550 copy from ReportGenerator 1.10.AllOS
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5C7FC2-4A79-4683-9486-884760C4552F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F598EA-3F6F-4115-B76B-AC4CB71E0447}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15435" tabRatio="701" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="234">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>BCID : name of the BCID to get the rule’s compounded weight and to filter results (60017 by default)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50</t>
   </si>
   <si>
     <t>* Block Name = AEFP_LIST</t>
@@ -892,27 +895,6 @@
   <si>
     <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
-  <si>
-    <t>UPDATED</t>
-  </si>
-  <si>
-    <r>
-      <t>CRITICITY =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> c for only critical violations, nc for only non critical violations, all for critical and non critical violations (all by default if not configured)</t>
-    </r>
-  </si>
-  <si>
-    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50,CRITICITY=all</t>
-  </si>
 </sst>
 </file>
 
@@ -921,7 +903,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1060,21 +1042,6 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1139,7 +1106,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1213,8 +1180,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1940,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,49 +1917,41 @@
     <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="I1" s="31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2018,12 +1975,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2033,37 +1990,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2071,27 +2028,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2116,12 +2073,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2131,17 +2088,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2154,7 +2111,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2170,7 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
   <dimension ref="B1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2182,12 +2139,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2154,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2210,7 +2167,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
REPORTGEN-596 : update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5C7FC2-4A79-4683-9486-884760C4552F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DFB12-646F-4FF0-8B90-B13C57132DF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="240">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -591,9 +591,6 @@
   </si>
   <si>
     <t>When you select the metric id for a BC or TC, all the QRs belonging to this BC or TC is added for displaying violations</t>
-  </si>
-  <si>
-    <t>3.8.	Evolution of sub-standards for a quality standard</t>
   </si>
   <si>
     <t>* Block Name = QUALITY_STANDARDS_EVOLUTION</t>
@@ -913,6 +910,79 @@
   <si>
     <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50,CRITICITY=all</t>
   </si>
+  <si>
+    <t>3.8.	Evolution of category or tag for a quality standard</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* MORE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* MORE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
+    </r>
+  </si>
+  <si>
+    <t>* LBL=violations or vulnerabilities (vulnerabilities if not set), this change the headers from Vulnerabilities to Violations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* MORE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -921,7 +991,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,6 +1145,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1139,7 +1230,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1198,6 +1289,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1213,8 +1306,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1619,8 +1711,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1631,16 +1723,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1688,26 +1780,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1732,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:B10"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,48 +1835,56 @@
     <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1808,42 +1908,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1851,12 +1951,12 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
@@ -1866,7 +1966,7 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1891,37 +1991,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1929,7 +2029,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1942,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
   <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,35 +2054,35 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>233</v>
+        <v>206</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>234</v>
+      <c r="B6" s="27" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1990,7 +2090,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2018,52 +2118,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2071,27 +2171,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2116,32 +2216,32 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2154,7 +2254,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2182,22 +2282,22 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2210,7 +2310,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -19824,7 +19924,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" s="24"/>
     </row>
@@ -19851,7 +19951,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-597 : updated library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DFB12-646F-4FF0-8B90-B13C57132DF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCEFA2-66DB-4C0B-B10C-885CA1E09283}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="3 - components by status list" sheetId="22" r:id="rId14"/>
     <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
     <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
+    <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="244">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -914,50 +915,6 @@
     <t>3.8.	Evolution of category or tag for a quality standard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* MORE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* MORE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
-    </r>
-  </si>
-  <si>
     <t>* LBL=violations or vulnerabilities (vulnerabilities if not set), this change the headers from Vulnerabilities to Violations</t>
   </si>
   <si>
@@ -983,6 +940,24 @@
       <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
     </r>
   </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>* Block Name = QUALITY_TAGS_RULES_EVOLUTION</t>
+  </si>
+  <si>
+    <t>* STD= Name of the quality standard category for which you want the details per tag, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
+  </si>
+  <si>
+    <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20190624</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=STIG-V4R8-CAT1</t>
+  </si>
+  <si>
+    <t>3.15.	Evolution of CAST rules associated to a quality standard category</t>
+  </si>
 </sst>
 </file>
 
@@ -991,7 +966,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1166,6 +1141,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1230,7 +1213,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1291,6 +1274,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1306,7 +1290,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1711,8 +1695,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1723,16 +1707,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1780,26 +1764,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1826,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
   <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,23 +1828,23 @@
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2315,6 +2299,72 @@
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-639 : add new component LIST_TAGS_DOC_BYCAT
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCEFA2-66DB-4C0B-B10C-885CA1E09283}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70D8F0-14A2-40FE-AC72-786AFF4B77EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
     <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
     <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
+    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="247">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -891,9 +892,6 @@
     <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
   <si>
-    <t>UPDATED</t>
-  </si>
-  <si>
     <r>
       <t>CRITICITY =</t>
     </r>
@@ -957,6 +955,18 @@
   </si>
   <si>
     <t>3.15.	Evolution of CAST rules associated to a quality standard category</t>
+  </si>
+  <si>
+    <t>* Block Name = LIST_TAGS_DOC_BYCAT</t>
+  </si>
+  <si>
+    <t>* CAT = Id of the standard quality category, for example, STIG-V4R8-CAT1, or a list separated by ‘|’</t>
+  </si>
+  <si>
+    <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20190909</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_TAGS_DOC_BYCAT;CAT=STIG-V4R8-CAT1</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1285,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1290,7 +1301,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1695,8 +1705,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1707,16 +1717,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1764,26 +1774,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1811,7 +1821,7 @@
   <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,11 +1831,9 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>232</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -1839,12 +1847,12 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2040,9 +2048,7 @@
       <c r="B1" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>232</v>
-      </c>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
@@ -2066,7 +2072,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2074,7 +2080,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2310,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,25 +2327,23 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>238</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2352,7 +2356,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2363,12 +2367,76 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
REPORTGEN-657: Add filter on ratio threshold for component TOP_COMPONENTS_BY_PROPERTIES
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70D8F0-14A2-40FE-AC72-786AFF4B77EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FCE157-BDB5-4046-9B71-9490A4D28ECE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="253">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -632,9 +632,6 @@
   </si>
   <si>
     <t>For PROP1 and PROP2, the available values are : codeLines, commentedCodeLines, commentLines, coupling, fanIn, fanOut, cyclomaticComplexity, ratioCommentLinesCodeLines, halsteadProgramLength, halsteadProgramVocabulary, halsteadVolume, distinctOperators, distinctOperands, integrationComplexity, essentialComplexity</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TOP_COMPONENTS_BY_PROPERTIES;PROP1=cyclomaticComplexity,PROP2=ratioCommentLinesCodeLines,ORDER1=desc,ORDER2=asc,COUNT=10</t>
   </si>
   <si>
     <t>If PROP1 and/or PROP2 is not correctly set,list of available values is displayed</t>
@@ -968,6 +965,27 @@
   <si>
     <t>RepGen:TABLE;LIST_TAGS_DOC_BYCAT;CAT=STIG-V4R8-CAT1</t>
   </si>
+  <si>
+    <t>LOWER1 : components should have prop1 value lower than this value</t>
+  </si>
+  <si>
+    <t>GREATER1 : components should have prop1 value greater than this value</t>
+  </si>
+  <si>
+    <t>LOWER2 : components should have prop2 value lower than this value</t>
+  </si>
+  <si>
+    <t>GREATER2 : components should have prop2 value greater than this value</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <t>When using LOWER and GREATER parameters, the ORDER parameter can be overridden to get the most accurate components corresponding to the request. As the filter can be done only after requesting data from the RestAPI, the list can be truncated. So the option NBSET define the number of objects returns from the rest api before the filtering and the limitation of display (COUNT), this option is set to 500 by default, to avoid too long server response time.</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TOP_COMPONENTS_BY_PROPERTIES;PROP1=cyclomaticComplexity,PROP2=ratioCommentLinesCodeLines,ORDER1=desc,ORDER2=asc,LOWER2=0.10,COUNT=100,NBSET=10000</t>
+  </si>
 </sst>
 </file>
 
@@ -976,7 +994,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1177,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1223,7 +1249,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1286,6 +1312,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1300,6 +1327,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1705,8 +1735,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1717,16 +1747,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1774,26 +1804,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1831,7 +1861,7 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C1" s="26"/>
     </row>
@@ -1847,12 +1877,12 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1887,78 +1917,112 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
-  <dimension ref="B1:B15"/>
+  <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="36" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1983,12 +2047,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -1998,22 +2062,22 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2021,7 +2085,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2046,13 +2110,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2062,17 +2126,17 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2080,7 +2144,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2108,12 +2172,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2123,37 +2187,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2161,27 +2225,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2206,12 +2270,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2221,17 +2285,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2244,7 +2308,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2272,12 +2336,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2351,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2300,7 +2364,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2327,23 +2391,23 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2356,7 +2420,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2367,7 +2431,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2380,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,22 +2454,22 @@
     <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>237</v>
+        <v>241</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2421,7 +2485,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,7 +2496,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -20042,7 +20106,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="24"/>
     </row>
@@ -20069,7 +20133,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>